<commit_message>
hexadecimal display works correctly
complement and horizontal inverse to get the correct output
</commit_message>
<xml_diff>
--- a/lab3/7 segment display.xlsx
+++ b/lab3/7 segment display.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\OneDrive\Documents\GitHub\ENSC-252\lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0722D5F4-7C25-4A7E-A54B-28BCC1A7975D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFCB61A-0046-4575-B451-908A25396F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="0" windowWidth="15165" windowHeight="15585" xr2:uid="{82B1C4A9-5616-4BE4-B8FF-7E380425325B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{82B1C4A9-5616-4BE4-B8FF-7E380425325B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>x1</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -134,10 +137,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,15 +474,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39200C3-6B46-4D71-AB94-0B9F019EE0DE}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41:N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="4.08984375" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="4.08984375" customWidth="1"/>
+    <col min="6" max="6" width="3.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -532,6 +536,18 @@
       <c r="B2">
         <v>0</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2">
         <v>1</v>
@@ -551,6 +567,9 @@
       <c r="M2">
         <v>1</v>
       </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -558,6 +577,15 @@
       </c>
       <c r="B3">
         <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -592,8 +620,17 @@
       <c r="B4">
         <v>2</v>
       </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
       <c r="E4">
         <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4">
@@ -625,6 +662,12 @@
       <c r="B5">
         <v>3</v>
       </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
       <c r="E5">
         <v>1</v>
       </c>
@@ -661,8 +704,17 @@
       <c r="B6">
         <v>4</v>
       </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
       <c r="D6">
         <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6">
@@ -694,8 +746,14 @@
       <c r="B7">
         <v>5</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
       <c r="D7">
         <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -730,6 +788,9 @@
       <c r="B8">
         <v>6</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
       <c r="D8">
         <v>1</v>
       </c>
@@ -769,6 +830,9 @@
       <c r="B9">
         <v>7</v>
       </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
       <c r="D9">
         <v>1</v>
       </c>
@@ -811,6 +875,15 @@
       <c r="C10">
         <v>1</v>
       </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10">
         <v>1</v>
@@ -844,6 +917,12 @@
       <c r="C11">
         <v>1</v>
       </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
       <c r="F11">
         <v>1</v>
       </c>
@@ -880,8 +959,14 @@
       <c r="C12">
         <v>1</v>
       </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
       <c r="E12">
         <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12">
@@ -916,6 +1001,9 @@
       <c r="C13">
         <v>1</v>
       </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
       <c r="E13">
         <v>1</v>
       </c>
@@ -958,6 +1046,12 @@
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14">
         <v>0</v>
@@ -994,6 +1088,9 @@
       <c r="D15">
         <v>1</v>
       </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
       <c r="F15">
         <v>1</v>
       </c>
@@ -1101,8 +1198,617 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="E18" s="2"/>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" t="s">
+        <v>7</v>
+      </c>
+      <c r="L25" t="s">
+        <v>6</v>
+      </c>
+      <c r="M25" t="s">
+        <v>5</v>
+      </c>
+      <c r="N25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>